<commit_message>
Jersey File upload and download
Jersey File upload and download
</commit_message>
<xml_diff>
--- a/requirements/requirements.xlsx
+++ b/requirements/requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="requiremens" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Bug Description and reproduce steps</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>File upload to controller instead of file name</t>
+  </si>
+  <si>
+    <t>Cerebro - Need utility to create page dynamically with entries i give</t>
+  </si>
+  <si>
+    <t>Update Cerebro with all core java example</t>
+  </si>
+  <si>
+    <t>Update Cerebro with core java definitions</t>
+  </si>
+  <si>
+    <t>Add Defintions web services -&gt; service factory -&gt; util class has 2 different method. But 2 methods are not needed, make it 1</t>
   </si>
 </sst>
 </file>
@@ -420,11 +432,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -480,6 +492,27 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -487,11 +520,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,6 +557,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>